<commit_message>
Bar charts based on Frequent Itemsets
Bar charts based on Frequent Itemsets have been added
</commit_message>
<xml_diff>
--- a/analysis/queryResults/FrequentItemsets_CA20022018.xlsx
+++ b/analysis/queryResults/FrequentItemsets_CA20022018.xlsx
@@ -30,279 +30,66 @@
     <t>count</t>
   </si>
   <si>
-    <t>{keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>sigAlg=\"SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{keySize=2048}</t>
   </si>
   <si>
-    <t>{keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A}</t>
   </si>
   <si>
-    <t>{rating=A,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=A,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A+}</t>
   </si>
   <si>
     <t>{rating=B}</t>
   </si>
   <si>
-    <t>{rating=A+,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=B,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=B,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=B,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=B,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=B,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=B,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=B,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A+,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=A+,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A-}</t>
   </si>
   <si>
-    <t>{rating=A-,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A-,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A-,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=A-,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=F}</t>
   </si>
   <si>
-    <t>{rating=F,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=C}</t>
   </si>
   <si>
-    <t>{rating=F,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=F,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=F,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=F,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=C,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=C,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=C,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=F,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=F,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=C,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=C,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=C,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=C,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{keySize=4096}</t>
   </si>
   <si>
-    <t>{keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=T}</t>
   </si>
   <si>
-    <t>{rating=T,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=T,keySize=2048}</t>
   </si>
   <si>
-    <t>{rating=T,keySize=2048,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{keyAlg=\EC\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=2048,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=2048,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=256,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
     <t>{keySize=256}</t>
   </si>
   <si>
-    <t>{sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>sigAlg=\"SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=256,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{keySize=256,sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=256,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
     <t>{rating=A,keySize=256}</t>
   </si>
   <si>
-    <t>{rating=A,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A,keySize=4096}</t>
   </si>
   <si>
-    <t>{rating=A,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{rating=A,sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=256,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{rating=A,keySize=256,sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A+,keySize=4096}</t>
   </si>
   <si>
-    <t>{rating=A+,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{keySize=null,keyAlg=null,sigAlg=null}</t>
   </si>
   <si>
@@ -324,33 +111,9 @@
     <t>{keySize=null}</t>
   </si>
   <si>
-    <t>sigAlg=\"SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=B,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=B,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=B,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=B,keySize=4096}</t>
   </si>
   <si>
-    <t>{keySize=2048,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A,keySize=null,keyAlg=null,sigAlg=null}</t>
   </si>
   <si>
@@ -372,24 +135,9 @@
     <t>{rating=A,keyAlg=null}</t>
   </si>
   <si>
-    <t>{rating=A+,keySize=256,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
     <t>{rating=A+,keySize=256}</t>
   </si>
   <si>
-    <t>{rating=T,keySize=2048,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A-,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=A-,keySize=4096}</t>
   </si>
   <si>
@@ -414,72 +162,18 @@
     <t>{rating=B,keyAlg=null}</t>
   </si>
   <si>
-    <t>{rating=C,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=C,keySize=4096}</t>
   </si>
   <si>
-    <t>{rating=C,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=C,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{rating=A+,sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=256,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=256,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=256,sigAlg=\SHA256withECDSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=F,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=T,keySize=4096}</t>
   </si>
   <si>
-    <t>{rating=F,keySize=4096,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=F,keySize=4096}</t>
   </si>
   <si>
-    <t>{rating=F,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=F,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=4096,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=4096,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=F,keySize=2048,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
     <t>{keySize=1024}</t>
   </si>
   <si>
-    <t>{keySize=1024,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=384,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
     <t>{keySize=384}</t>
   </si>
   <si>
@@ -525,27 +219,9 @@
     <t>{rating=F,keyAlg=null}</t>
   </si>
   <si>
-    <t>{rating=A,keySize=256,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{keySize=384,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{keySize=384,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=384,keyAlg=\EC\"}"</t>
-  </si>
-  <si>
     <t>{rating=A+,keySize=384}</t>
   </si>
   <si>
-    <t>{keySize=1024,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{keySize=1024,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=C,keySize=null,keyAlg=null,sigAlg=null}</t>
   </si>
   <si>
@@ -588,21 +264,9 @@
     <t>{rating=A-,keyAlg=null}</t>
   </si>
   <si>
-    <t>{rating=A+,keySize=384,keyAlg=\EC\"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=384,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{rating=A+,keySize=256,sigAlg=\SHA256withRSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=T,keySize=1024}</t>
   </si>
   <si>
-    <t>{rating=T,keySize=1024,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=T,keySize=null,keyAlg=null,sigAlg=null}</t>
   </si>
   <si>
@@ -624,22 +288,358 @@
     <t>{rating=T,keyAlg=null}</t>
   </si>
   <si>
-    <t>{rating=F,keySize=1024,keyAlg=\RSA\"}"</t>
-  </si>
-  <si>
     <t>{rating=F,keySize=1024}</t>
   </si>
   <si>
-    <t>{rating=T,keySize=1024,keyAlg=\RSA\"</t>
-  </si>
-  <si>
-    <t>{rating=T,keySize=1024,sigAlg=\SHA1withRSA\"}"</t>
-  </si>
-  <si>
-    <t>sigAlg=\"SHA512withRSA\"}"</t>
-  </si>
-  <si>
-    <t>{sigAlg=\SHA512withRSA\"}"</t>
+    <t>{sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=B,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=2048,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=256,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=4096,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=256,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=384,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=384,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=256,sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>sigAlg=\"SHA512withRSA\"}</t>
+  </si>
+  <si>
+    <t>{keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A+,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=B,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=B,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A-,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=F,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=T,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=2048,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=2048,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=B,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=A-,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=C,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=4096,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=4096,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{keySize=1024,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{keySize=1024,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=1024,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=1024,keyAlg=RSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=1024,keyAlg=RSA</t>
+  </si>
+  <si>
+    <t>{sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{keySize=256,sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=256,sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=256,sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>{keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{keySize=256,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{keySize=256,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{rating=A,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=256,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{rating=A,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{rating=A,keySize=256,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{rating=A+,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=256,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=256,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{keySize=384,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{keySize=384,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=384,keyAlg=EC}</t>
+  </si>
+  <si>
+    <t>{rating=A+,keySize=384,keyAlg=EC</t>
+  </si>
+  <si>
+    <t>sigAlg=SHA256withECDSA}</t>
+  </si>
+  <si>
+    <t>sigAlg=SHA256withRSA}</t>
+  </si>
+  <si>
+    <t>sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=2048,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=2048,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=F,keySize=2048,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{keySize=1024,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{rating=T,keySize=1024,sigAlg=SHA1withRSA}</t>
+  </si>
+  <si>
+    <t>{sigAlg=SHA512withRSA}</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -986,6 +986,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1147,13 +1153,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1210,6 +1217,951 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Key</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Signature Algorithm Distributions</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(FrequentItemsets_CA20022018!$B$3,FrequentItemsets_CA20022018!$B$72,FrequentItemsets_CA20022018!$B$96,FrequentItemsets_CA20022018!$B$99,FrequentItemsets_CA20022018!$B$214)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>{sigAlg=SHA256withRSA}</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>{sigAlg=SHA256withECDSA}</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>{sigAlg=null}</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>{sigAlg=SHA1withRSA}</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>{sigAlg=SHA512withRSA}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(FrequentItemsets_CA20022018!$C$3,FrequentItemsets_CA20022018!$C$72,FrequentItemsets_CA20022018!$C$96,FrequentItemsets_CA20022018!$C$99,FrequentItemsets_CA20022018!$C$214)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.93267093206094498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3495092989210003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.14580057474381E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.04104538307217E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.11153283088435E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2096246768"/>
+        <c:axId val="2096245680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2096246768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2096245680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2096245680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2096246768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295104</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>580854</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>17008</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1477,8 +2429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152:E152"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +2456,7 @@
         <v>193</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1">
         <v>0.938120153987963</v>
@@ -1514,16 +2466,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>194</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="6">
         <v>0.93267093206094498</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>68805</v>
       </c>
     </row>
@@ -1532,10 +2484,10 @@
         <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D4" s="2">
         <v>0.92586618229138395</v>
@@ -1549,7 +2501,7 @@
         <v>195</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5">
         <v>0.85699181261183099</v>
@@ -1564,7 +2516,7 @@
         <v>190</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2">
         <v>0.85697825733340605</v>
@@ -1579,10 +2531,10 @@
         <v>189</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2">
         <v>0.84797755245892703</v>
@@ -1596,7 +2548,7 @@
         <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C8">
         <v>0.84797755245892703</v>
@@ -1610,7 +2562,7 @@
         <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>0.39661389144933001</v>
@@ -1624,7 +2576,7 @@
         <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>0.36153283088434601</v>
@@ -1638,7 +2590,7 @@
         <v>186</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1">
         <v>0.35876755408556099</v>
@@ -1653,10 +2605,10 @@
         <v>185</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D12" s="1">
         <v>0.35842867212492502</v>
@@ -1670,7 +2622,7 @@
         <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1">
         <v>0.32950170796508199</v>
@@ -1685,7 +2637,7 @@
         <v>188</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C14" s="5">
         <v>0.32950170796508199</v>
@@ -1700,10 +2652,10 @@
         <v>182</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D15" s="1">
         <v>0.32925771295342399</v>
@@ -1717,7 +2669,7 @@
         <v>184</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C16" s="5">
         <v>0.32925771295342399</v>
@@ -1732,7 +2684,7 @@
         <v>197</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>0.14326573767825199</v>
@@ -1746,7 +2698,7 @@
         <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>0.13658298541451999</v>
@@ -1760,7 +2712,7 @@
         <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="C19">
         <v>0.13597299788537701</v>
@@ -1774,7 +2726,7 @@
         <v>179</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="C20" s="1">
         <v>0.13267906522799999</v>
@@ -1789,10 +2741,10 @@
         <v>178</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D21" s="1">
         <v>0.132597733557447</v>
@@ -1806,7 +2758,7 @@
         <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>0.13156753239711499</v>
@@ -1820,7 +2772,7 @@
         <v>172</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1">
         <v>0.131459090169712</v>
@@ -1835,10 +2787,10 @@
         <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D24" s="1">
         <v>0.131364203220734</v>
@@ -1852,7 +2804,7 @@
         <v>169</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1">
         <v>0.12251260640893601</v>
@@ -1867,7 +2819,7 @@
         <v>174</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5">
         <v>0.12251260640893601</v>
@@ -1882,10 +2834,10 @@
         <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D27" s="1">
         <v>0.122417719459958</v>
@@ -1899,7 +2851,7 @@
         <v>170</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="C28" s="5">
         <v>0.122417719459958</v>
@@ -1914,7 +2866,7 @@
         <v>176</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="C29" s="1">
         <v>0.110150192484954</v>
@@ -1929,7 +2881,7 @@
         <v>181</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C30" s="5">
         <v>0.110150192484954</v>
@@ -1944,10 +2896,10 @@
         <v>175</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D31" s="1">
         <v>0.11010952664967701</v>
@@ -1961,7 +2913,7 @@
         <v>177</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C32" s="5">
         <v>0.11010952664967701</v>
@@ -1976,7 +2928,7 @@
         <v>199</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C33">
         <v>9.8235102749010497E-2</v>
@@ -1990,7 +2942,7 @@
         <v>165</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1">
         <v>9.6418695440004296E-2</v>
@@ -2005,10 +2957,10 @@
         <v>164</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D35" s="1">
         <v>9.6323808491026397E-2</v>
@@ -2022,7 +2974,7 @@
         <v>166</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C36">
         <v>9.6323808491026397E-2</v>
@@ -2036,7 +2988,7 @@
         <v>162</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="C37" s="1">
         <v>9.1227023803068893E-2</v>
@@ -2051,7 +3003,7 @@
         <v>167</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C38" s="5">
         <v>9.1227023803068893E-2</v>
@@ -2066,10 +3018,10 @@
         <v>161</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D39" s="1">
         <v>9.1132136854090995E-2</v>
@@ -2083,7 +3035,7 @@
         <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="C40">
         <v>9.1132136854090995E-2</v>
@@ -2097,7 +3049,7 @@
         <v>200</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>9.0657702109201294E-2</v>
@@ -2111,7 +3063,7 @@
         <v>158</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="C42" s="1">
         <v>8.8000867537819202E-2</v>
@@ -2126,7 +3078,7 @@
         <v>201</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="C43">
         <v>8.3703844276961495E-2</v>
@@ -2140,7 +3092,7 @@
         <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>8.3432738708453094E-2</v>
@@ -2154,10 +3106,10 @@
         <v>157</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D45" s="1">
         <v>8.3419183430027605E-2</v>
@@ -2171,7 +3123,7 @@
         <v>155</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1">
         <v>8.2904082849861699E-2</v>
@@ -2186,7 +3138,7 @@
         <v>160</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C47" s="5">
         <v>8.2904082849861699E-2</v>
@@ -2201,7 +3153,7 @@
         <v>151</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="C48" s="1">
         <v>8.1656997234723194E-2</v>
@@ -2216,7 +3168,7 @@
         <v>152</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>8.1616331399446906E-2</v>
@@ -2230,10 +3182,10 @@
         <v>150</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D50" s="1">
         <v>8.16027761210215E-2</v>
@@ -2247,10 +3199,10 @@
         <v>154</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D51" s="1">
         <v>7.9786368812015396E-2</v>
@@ -2264,7 +3216,7 @@
         <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="C52">
         <v>7.9786368812015396E-2</v>
@@ -2278,7 +3230,7 @@
         <v>148</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1">
         <v>7.6885539228975799E-2</v>
@@ -2293,7 +3245,7 @@
         <v>153</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C54" s="5">
         <v>7.6885539228975799E-2</v>
@@ -2308,10 +3260,10 @@
         <v>147</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D55" s="1">
         <v>7.6844873393699498E-2</v>
@@ -2325,7 +3277,7 @@
         <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="C56">
         <v>7.6844873393699498E-2</v>
@@ -2339,7 +3291,7 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="C57">
         <v>7.6817762836848699E-2</v>
@@ -2353,7 +3305,7 @@
         <v>202</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C58" s="4">
         <v>7.6817762836848699E-2</v>
@@ -2368,10 +3320,10 @@
         <v>138</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D59" s="4">
         <v>7.6180664750853999E-2</v>
@@ -2385,7 +3337,7 @@
         <v>140</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="C60" s="4">
         <v>7.6180664750853999E-2</v>
@@ -2400,7 +3352,7 @@
         <v>203</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="C61">
         <v>5.0940736322724098E-2</v>
@@ -2414,7 +3366,7 @@
         <v>116</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="C62" s="1">
         <v>4.9137884292143399E-2</v>
@@ -2428,7 +3380,7 @@
         <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C63">
         <v>4.38106598709537E-2</v>
@@ -2442,7 +3394,7 @@
         <v>113</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="C64" s="1">
         <v>4.3797104592528301E-2</v>
@@ -2456,7 +3408,7 @@
         <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="C65">
         <v>4.2224692295179701E-2</v>
@@ -2470,10 +3422,10 @@
         <v>115</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D66" s="1">
         <v>4.2129805346201803E-2</v>
@@ -2487,7 +3439,7 @@
         <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="C67">
         <v>4.0394729707748198E-2</v>
@@ -2501,10 +3453,10 @@
         <v>112</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D68" s="1">
         <v>3.84292143360625E-2</v>
@@ -2518,7 +3470,7 @@
         <v>114</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="C69">
         <v>3.84292143360625E-2</v>
@@ -2532,7 +3484,7 @@
         <v>103</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="C70">
         <v>3.7412568454155998E-2</v>
@@ -2546,7 +3498,7 @@
         <v>205</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>3.7412568454155998E-2</v>
@@ -2556,16 +3508,16 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="6">
         <v>206</v>
       </c>
-      <c r="B72" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72">
+      <c r="B72" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" s="6">
         <v>3.3495092989210003E-2</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="6">
         <v>2471</v>
       </c>
     </row>
@@ -2574,10 +3526,10 @@
         <v>91</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>75</v>
+        <v>181</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D73" s="3">
         <v>3.3481537710784597E-2</v>
@@ -2591,10 +3543,10 @@
         <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="C74" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D74">
         <v>3.2952881852193201E-2</v>
@@ -2608,7 +3560,7 @@
         <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>174</v>
       </c>
       <c r="C75">
         <v>3.2952881852193201E-2</v>
@@ -2622,7 +3574,7 @@
         <v>107</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="C76" s="3">
         <v>3.1760017350756398E-2</v>
@@ -2636,7 +3588,7 @@
         <v>96</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="C77" s="3">
         <v>3.1041587594209202E-2</v>
@@ -2650,7 +3602,7 @@
         <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C78">
         <v>3.1041587594209202E-2</v>
@@ -2664,7 +3616,7 @@
         <v>136</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="C79" s="1">
         <v>2.8832077210865899E-2</v>
@@ -2678,7 +3630,7 @@
         <v>141</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="C80" s="4">
         <v>2.8832077210865899E-2</v>
@@ -2693,10 +3645,10 @@
         <v>135</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D81" s="1">
         <v>2.8737190261888E-2</v>
@@ -2710,7 +3662,7 @@
         <v>137</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C82" s="4">
         <v>2.8737190261888E-2</v>
@@ -2725,10 +3677,10 @@
         <v>87</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D83" s="3">
         <v>2.8615192756059199E-2</v>
@@ -2742,7 +3694,7 @@
         <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
+        <v>175</v>
       </c>
       <c r="C84">
         <v>2.8615192756059199E-2</v>
@@ -2756,10 +3708,10 @@
         <v>82</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D85" s="3">
         <v>2.85203058070813E-2</v>
@@ -2773,7 +3725,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="C86">
         <v>2.85203058070813E-2</v>
@@ -2787,7 +3739,7 @@
         <v>133</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="C87" s="4">
         <v>2.2284877731388601E-2</v>
@@ -2802,7 +3754,7 @@
         <v>142</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="C88" s="4">
         <v>2.2284877731388601E-2</v>
@@ -2817,10 +3769,10 @@
         <v>132</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>92</v>
+        <v>157</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D89" s="4">
         <v>2.2244211896112299E-2</v>
@@ -2834,7 +3786,7 @@
         <v>134</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C90" s="4">
         <v>2.2244211896112299E-2</v>
@@ -2849,7 +3801,7 @@
         <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="C91">
         <v>2.14580057474381E-2</v>
@@ -2863,7 +3815,7 @@
         <v>58</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="C92">
         <v>2.14580057474381E-2</v>
@@ -2877,7 +3829,7 @@
         <v>59</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="C93">
         <v>2.14580057474381E-2</v>
@@ -2891,7 +3843,7 @@
         <v>74</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="C94">
         <v>2.14580057474381E-2</v>
@@ -2905,7 +3857,7 @@
         <v>207</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="C95">
         <v>2.14580057474381E-2</v>
@@ -2915,16 +3867,16 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="6">
         <v>208</v>
       </c>
-      <c r="B96" t="s">
-        <v>99</v>
-      </c>
-      <c r="C96">
+      <c r="B96" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="6">
         <v>2.14580057474381E-2</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="6">
         <v>1583</v>
       </c>
     </row>
@@ -2933,7 +3885,7 @@
         <v>209</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="C97">
         <v>2.14580057474381E-2</v>
@@ -2947,10 +3899,10 @@
         <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D98">
         <v>1.04104538307217E-2</v>
@@ -2960,16 +3912,16 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="A99" s="6">
         <v>210</v>
       </c>
-      <c r="B99" t="s">
-        <v>102</v>
-      </c>
-      <c r="C99">
+      <c r="B99" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C99" s="6">
         <v>1.04104538307217E-2</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="6">
         <v>768</v>
       </c>
     </row>
@@ -2978,10 +3930,10 @@
         <v>129</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D100" s="4">
         <v>8.7160440275443306E-3</v>
@@ -2995,7 +3947,7 @@
         <v>130</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="C101" s="4">
         <v>8.7160440275443306E-3</v>
@@ -3010,7 +3962,7 @@
         <v>131</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C102" s="4">
         <v>8.7160440275443306E-3</v>
@@ -3025,7 +3977,7 @@
         <v>143</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="C103" s="4">
         <v>8.7160440275443306E-3</v>
@@ -3040,10 +3992,10 @@
         <v>24</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D104">
         <v>8.0925012199750592E-3</v>
@@ -3057,7 +4009,7 @@
         <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>199</v>
       </c>
       <c r="C105">
         <v>8.0925012199750592E-3</v>
@@ -3071,7 +4023,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="C106">
         <v>7.9027273220191908E-3</v>
@@ -3085,10 +4037,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>75</v>
+        <v>181</v>
       </c>
       <c r="C107" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D107">
         <v>6.8047497695602702E-3</v>
@@ -3102,10 +4054,10 @@
         <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="C108" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D108">
         <v>6.3980914167977004E-3</v>
@@ -3119,7 +4071,7 @@
         <v>28</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
       <c r="C109">
         <v>6.3980914167977004E-3</v>
@@ -3133,7 +4085,7 @@
         <v>29</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="C110">
         <v>6.0863200130130699E-3</v>
@@ -3147,7 +4099,7 @@
         <v>36</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C111">
         <v>6.0863200130130699E-3</v>
@@ -3161,7 +4113,7 @@
         <v>44</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="C112">
         <v>6.0863200130130699E-3</v>
@@ -3175,7 +4127,7 @@
         <v>51</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>34</v>
       </c>
       <c r="C113">
         <v>6.0863200130130699E-3</v>
@@ -3189,7 +4141,7 @@
         <v>60</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="C114">
         <v>6.0863200130130699E-3</v>
@@ -3203,7 +4155,7 @@
         <v>67</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="C115">
         <v>6.0863200130130699E-3</v>
@@ -3217,7 +4169,7 @@
         <v>75</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="C116">
         <v>6.0863200130130699E-3</v>
@@ -3231,7 +4183,7 @@
         <v>97</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>117</v>
+        <v>188</v>
       </c>
       <c r="C117" s="3">
         <v>5.7474380523776002E-3</v>
@@ -3245,7 +4197,7 @@
         <v>102</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C118">
         <v>5.7474380523776002E-3</v>
@@ -3259,10 +4211,10 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="C119" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D119">
         <v>5.1103399663829097E-3</v>
@@ -3276,7 +4228,7 @@
         <v>20</v>
       </c>
       <c r="B120" t="s">
-        <v>119</v>
+        <v>201</v>
       </c>
       <c r="C120">
         <v>5.1103399663829097E-3</v>
@@ -3290,10 +4242,10 @@
         <v>126</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D121" s="4">
         <v>5.0967846879574896E-3</v>
@@ -3307,7 +4259,7 @@
         <v>127</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="C122" s="4">
         <v>5.0967846879574896E-3</v>
@@ -3322,7 +4274,7 @@
         <v>128</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C123" s="4">
         <v>5.0967846879574896E-3</v>
@@ -3337,7 +4289,7 @@
         <v>144</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="C124" s="4">
         <v>5.0967846879574896E-3</v>
@@ -3352,7 +4304,7 @@
         <v>31</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C125">
         <v>4.8799002331507899E-3</v>
@@ -3366,7 +4318,7 @@
         <v>38</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C126">
         <v>4.8799002331507899E-3</v>
@@ -3380,7 +4332,7 @@
         <v>46</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="C127">
         <v>4.8799002331507899E-3</v>
@@ -3394,7 +4346,7 @@
         <v>53</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="C128">
         <v>4.8799002331507899E-3</v>
@@ -3408,7 +4360,7 @@
         <v>62</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
+        <v>44</v>
       </c>
       <c r="C129">
         <v>4.8799002331507899E-3</v>
@@ -3422,7 +4374,7 @@
         <v>69</v>
       </c>
       <c r="B130" t="s">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="C130">
         <v>4.8799002331507899E-3</v>
@@ -3436,7 +4388,7 @@
         <v>77</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="C131">
         <v>4.8799002331507899E-3</v>
@@ -3450,7 +4402,7 @@
         <v>121</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="C132" s="4">
         <v>4.7172368920457598E-3</v>
@@ -3465,7 +4417,7 @@
         <v>146</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="C133" s="4">
         <v>4.7172368920457598E-3</v>
@@ -3480,10 +4432,10 @@
         <v>120</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D134" s="4">
         <v>4.7036816136203398E-3</v>
@@ -3497,7 +4449,7 @@
         <v>122</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="C135" s="4">
         <v>4.7036816136203398E-3</v>
@@ -3512,10 +4464,10 @@
         <v>88</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D136" s="3">
         <v>4.5139077156644801E-3</v>
@@ -3529,7 +4481,7 @@
         <v>90</v>
       </c>
       <c r="B137" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="C137">
         <v>4.5139077156644801E-3</v>
@@ -3543,10 +4495,10 @@
         <v>95</v>
       </c>
       <c r="B138" t="s">
-        <v>77</v>
+        <v>182</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D138">
         <v>4.4054654882611302E-3</v>
@@ -3560,7 +4512,7 @@
         <v>100</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="C139">
         <v>4.4054654882611302E-3</v>
@@ -3574,10 +4526,10 @@
         <v>83</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="D140" s="3">
         <v>4.1208046413273303E-3</v>
@@ -3591,7 +4543,7 @@
         <v>85</v>
       </c>
       <c r="B141" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="C141">
         <v>4.1208046413273303E-3</v>
@@ -3605,10 +4557,10 @@
         <v>22</v>
       </c>
       <c r="B142" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="C142" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D142">
         <v>4.0123624139239804E-3</v>
@@ -3622,7 +4574,7 @@
         <v>27</v>
       </c>
       <c r="B143" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="C143">
         <v>4.0123624139239804E-3</v>
@@ -3636,7 +4588,7 @@
         <v>110</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="C144" s="4">
         <v>3.6463698964376702E-3</v>
@@ -3651,7 +4603,7 @@
         <v>119</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>142</v>
+        <v>48</v>
       </c>
       <c r="C145" s="4">
         <v>3.6463698964376702E-3</v>
@@ -3666,7 +4618,7 @@
         <v>124</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="C146" s="4">
         <v>3.5243723906088998E-3</v>
@@ -3681,7 +4633,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>144</v>
+        <v>49</v>
       </c>
       <c r="C147" s="4">
         <v>3.5243723906088998E-3</v>
@@ -3696,10 +4648,10 @@
         <v>123</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D148" s="4">
         <v>3.42948544163097E-3</v>
@@ -3713,7 +4665,7 @@
         <v>125</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C149" s="4">
         <v>3.42948544163097E-3</v>
@@ -3728,10 +4680,10 @@
         <v>104</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D150" s="3">
         <v>3.3752643279292998E-3</v>
@@ -3745,10 +4697,10 @@
         <v>109</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D151" s="1">
         <v>3.2532668221005299E-3</v>
@@ -3762,7 +4714,7 @@
         <v>111</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C152" s="4">
         <v>3.2532668221005299E-3</v>
@@ -3777,10 +4729,10 @@
         <v>105</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D153" s="3">
         <v>3.1041587594209199E-3</v>
@@ -3794,10 +4746,10 @@
         <v>21</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D154" s="1">
         <v>2.98216125359215E-3</v>
@@ -3811,7 +4763,7 @@
         <v>23</v>
       </c>
       <c r="B155" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
       <c r="C155">
         <v>2.98216125359215E-3</v>
@@ -3825,7 +4777,7 @@
         <v>211</v>
       </c>
       <c r="B156" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C156">
         <v>2.98216125359215E-3</v>
@@ -3839,7 +4791,7 @@
         <v>14</v>
       </c>
       <c r="B157" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="C157">
         <v>2.9686059751667299E-3</v>
@@ -3853,7 +4805,7 @@
         <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="C158">
         <v>2.9008295830396402E-3</v>
@@ -3867,7 +4819,7 @@
         <v>212</v>
       </c>
       <c r="B159" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="C159">
         <v>2.9008295830396402E-3</v>
@@ -3881,7 +4833,7 @@
         <v>30</v>
       </c>
       <c r="B160" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="C160">
         <v>2.68394512823293E-3</v>
@@ -3895,7 +4847,7 @@
         <v>37</v>
       </c>
       <c r="B161" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="C161">
         <v>2.68394512823293E-3</v>
@@ -3909,7 +4861,7 @@
         <v>45</v>
       </c>
       <c r="B162" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="C162">
         <v>2.68394512823293E-3</v>
@@ -3923,7 +4875,7 @@
         <v>52</v>
       </c>
       <c r="B163" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="C163">
         <v>2.68394512823293E-3</v>
@@ -3937,7 +4889,7 @@
         <v>61</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>56</v>
       </c>
       <c r="C164">
         <v>2.68394512823293E-3</v>
@@ -3951,7 +4903,7 @@
         <v>68</v>
       </c>
       <c r="B165" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="C165">
         <v>2.68394512823293E-3</v>
@@ -3965,7 +4917,7 @@
         <v>76</v>
       </c>
       <c r="B166" t="s">
-        <v>160</v>
+        <v>58</v>
       </c>
       <c r="C166">
         <v>2.68394512823293E-3</v>
@@ -3979,7 +4931,7 @@
         <v>33</v>
       </c>
       <c r="B167" t="s">
-        <v>161</v>
+        <v>59</v>
       </c>
       <c r="C167">
         <v>2.53483706555333E-3</v>
@@ -3993,7 +4945,7 @@
         <v>40</v>
       </c>
       <c r="B168" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
       <c r="C168">
         <v>2.53483706555333E-3</v>
@@ -4007,7 +4959,7 @@
         <v>48</v>
       </c>
       <c r="B169" t="s">
-        <v>163</v>
+        <v>61</v>
       </c>
       <c r="C169">
         <v>2.53483706555333E-3</v>
@@ -4021,7 +4973,7 @@
         <v>55</v>
       </c>
       <c r="B170" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="C170">
         <v>2.53483706555333E-3</v>
@@ -4035,7 +4987,7 @@
         <v>64</v>
       </c>
       <c r="B171" t="s">
-        <v>165</v>
+        <v>63</v>
       </c>
       <c r="C171">
         <v>2.53483706555333E-3</v>
@@ -4049,7 +5001,7 @@
         <v>71</v>
       </c>
       <c r="B172" t="s">
-        <v>166</v>
+        <v>64</v>
       </c>
       <c r="C172">
         <v>2.53483706555333E-3</v>
@@ -4063,7 +5015,7 @@
         <v>79</v>
       </c>
       <c r="B173" t="s">
-        <v>167</v>
+        <v>65</v>
       </c>
       <c r="C173">
         <v>2.53483706555333E-3</v>
@@ -4077,10 +5029,10 @@
         <v>94</v>
       </c>
       <c r="B174" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
       <c r="C174" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D174">
         <v>2.4806159518516498E-3</v>
@@ -4094,7 +5046,7 @@
         <v>99</v>
       </c>
       <c r="B175" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
       <c r="C175">
         <v>2.4806159518516498E-3</v>
@@ -4108,10 +5060,10 @@
         <v>3</v>
       </c>
       <c r="B176" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="C176" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D176">
         <v>2.39928428129914E-3</v>
@@ -4125,7 +5077,7 @@
         <v>6</v>
       </c>
       <c r="B177" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="C177">
         <v>2.39928428129914E-3</v>
@@ -4139,7 +5091,7 @@
         <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="C178">
         <v>2.0875128775145E-3</v>
@@ -4153,7 +5105,7 @@
         <v>7</v>
       </c>
       <c r="B179" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="C179">
         <v>2.0875128775145E-3</v>
@@ -4167,10 +5119,10 @@
         <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C180" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D180">
         <v>2.0739575990890899E-3</v>
@@ -4184,7 +5136,7 @@
         <v>17</v>
       </c>
       <c r="B181" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="C181">
         <v>2.0739575990890899E-3</v>
@@ -4198,7 +5150,7 @@
         <v>34</v>
       </c>
       <c r="B182" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
       <c r="C182">
         <v>2.0061812069619902E-3</v>
@@ -4212,7 +5164,7 @@
         <v>41</v>
       </c>
       <c r="B183" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="C183">
         <v>2.0061812069619902E-3</v>
@@ -4226,7 +5178,7 @@
         <v>49</v>
       </c>
       <c r="B184" t="s">
-        <v>177</v>
+        <v>69</v>
       </c>
       <c r="C184">
         <v>2.0061812069619902E-3</v>
@@ -4240,7 +5192,7 @@
         <v>56</v>
       </c>
       <c r="B185" t="s">
-        <v>178</v>
+        <v>70</v>
       </c>
       <c r="C185">
         <v>2.0061812069619902E-3</v>
@@ -4254,7 +5206,7 @@
         <v>65</v>
       </c>
       <c r="B186" t="s">
-        <v>179</v>
+        <v>71</v>
       </c>
       <c r="C186">
         <v>2.0061812069619902E-3</v>
@@ -4268,7 +5220,7 @@
         <v>72</v>
       </c>
       <c r="B187" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="C187">
         <v>2.0061812069619902E-3</v>
@@ -4282,7 +5234,7 @@
         <v>80</v>
       </c>
       <c r="B188" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="C188">
         <v>2.0061812069619902E-3</v>
@@ -4296,7 +5248,7 @@
         <v>32</v>
       </c>
       <c r="B189" t="s">
-        <v>182</v>
+        <v>74</v>
       </c>
       <c r="C189">
         <v>1.77574147372987E-3</v>
@@ -4310,7 +5262,7 @@
         <v>39</v>
       </c>
       <c r="B190" t="s">
-        <v>183</v>
+        <v>75</v>
       </c>
       <c r="C190">
         <v>1.77574147372987E-3</v>
@@ -4324,7 +5276,7 @@
         <v>47</v>
       </c>
       <c r="B191" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="C191">
         <v>1.77574147372987E-3</v>
@@ -4338,7 +5290,7 @@
         <v>54</v>
       </c>
       <c r="B192" t="s">
-        <v>185</v>
+        <v>77</v>
       </c>
       <c r="C192">
         <v>1.77574147372987E-3</v>
@@ -4352,7 +5304,7 @@
         <v>63</v>
       </c>
       <c r="B193" t="s">
-        <v>186</v>
+        <v>78</v>
       </c>
       <c r="C193">
         <v>1.77574147372987E-3</v>
@@ -4366,7 +5318,7 @@
         <v>70</v>
       </c>
       <c r="B194" t="s">
-        <v>187</v>
+        <v>79</v>
       </c>
       <c r="C194">
         <v>1.77574147372987E-3</v>
@@ -4380,7 +5332,7 @@
         <v>78</v>
       </c>
       <c r="B195" t="s">
-        <v>188</v>
+        <v>80</v>
       </c>
       <c r="C195">
         <v>1.77574147372987E-3</v>
@@ -4394,10 +5346,10 @@
         <v>2</v>
       </c>
       <c r="B196" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C196" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D196">
         <v>1.7486309168790301E-3</v>
@@ -4411,7 +5363,7 @@
         <v>5</v>
       </c>
       <c r="B197" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="C197">
         <v>1.7486309168790301E-3</v>
@@ -4425,10 +5377,10 @@
         <v>93</v>
       </c>
       <c r="B198" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="C198" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="D198">
         <v>1.62663341105026E-3</v>
@@ -4442,7 +5394,7 @@
         <v>98</v>
       </c>
       <c r="B199" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
       <c r="C199">
         <v>1.62663341105026E-3</v>
@@ -4456,7 +5408,7 @@
         <v>16</v>
       </c>
       <c r="B200" t="s">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="C200">
         <v>1.57241229734859E-3</v>
@@ -4470,7 +5422,7 @@
         <v>12</v>
       </c>
       <c r="B201" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="C201">
         <v>1.55885701892317E-3</v>
@@ -4484,7 +5436,7 @@
         <v>35</v>
       </c>
       <c r="B202" t="s">
-        <v>194</v>
+        <v>82</v>
       </c>
       <c r="C202">
         <v>1.49108062679607E-3</v>
@@ -4498,7 +5450,7 @@
         <v>42</v>
       </c>
       <c r="B203" t="s">
-        <v>195</v>
+        <v>83</v>
       </c>
       <c r="C203">
         <v>1.49108062679607E-3</v>
@@ -4512,7 +5464,7 @@
         <v>50</v>
       </c>
       <c r="B204" t="s">
-        <v>196</v>
+        <v>84</v>
       </c>
       <c r="C204">
         <v>1.49108062679607E-3</v>
@@ -4526,7 +5478,7 @@
         <v>57</v>
       </c>
       <c r="B205" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
       <c r="C205">
         <v>1.49108062679607E-3</v>
@@ -4540,7 +5492,7 @@
         <v>66</v>
       </c>
       <c r="B206" t="s">
-        <v>198</v>
+        <v>86</v>
       </c>
       <c r="C206">
         <v>1.49108062679607E-3</v>
@@ -4554,7 +5506,7 @@
         <v>73</v>
       </c>
       <c r="B207" t="s">
-        <v>199</v>
+        <v>87</v>
       </c>
       <c r="C207">
         <v>1.49108062679607E-3</v>
@@ -4568,7 +5520,7 @@
         <v>81</v>
       </c>
       <c r="B208" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="C208">
         <v>1.49108062679607E-3</v>
@@ -4582,7 +5534,7 @@
         <v>13</v>
       </c>
       <c r="B209" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="C209">
         <v>1.40974895624356E-3</v>
@@ -4596,7 +5548,7 @@
         <v>15</v>
       </c>
       <c r="B210" t="s">
-        <v>202</v>
+        <v>89</v>
       </c>
       <c r="C210">
         <v>1.40974895624356E-3</v>
@@ -4610,10 +5562,10 @@
         <v>9</v>
       </c>
       <c r="B211" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="C211" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="D211">
         <v>1.12508810930977E-3</v>
@@ -4627,7 +5579,7 @@
         <v>11</v>
       </c>
       <c r="B212" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C212">
         <v>1.12508810930977E-3</v>
@@ -4641,10 +5593,10 @@
         <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="C213" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="D213">
         <v>1.11153283088435E-3</v>
@@ -4654,20 +5606,21 @@
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214">
+      <c r="A214" s="6">
         <v>213</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="6">
         <v>1.11153283088435E-3</v>
       </c>
-      <c r="D214">
+      <c r="D214" s="6">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After removing null, err and changing color
After removing null, err and changing color
</commit_message>
<xml_diff>
--- a/analysis/queryResults/FrequentItemsets_CA20022018.xlsx
+++ b/analysis/queryResults/FrequentItemsets_CA20022018.xlsx
@@ -1258,7 +1258,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Signature Algorithm Distributions</a:t>
+              <a:t> Signature Algorithms Distribution</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1431,11 +1431,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2096246768"/>
-        <c:axId val="2096245680"/>
+        <c:axId val="-1381979920"/>
+        <c:axId val="-1381976112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096246768"/>
+        <c:axId val="-1381979920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096245680"/>
+        <c:crossAx val="-1381976112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2096245680"/>
+        <c:axId val="-1381976112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,7 +1537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096246768"/>
+        <c:crossAx val="-1381979920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1581,7 +1581,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>

</xml_diff>